<commit_message>
benefit priority is now function of its own. wealth test is done for all benefits within `benefit_priority()`. tests had to be adjusted.
Former-commit-id: 802c2a72f5dc6c7b2a527e91c4743ef20caf4c0a
Former-commit-id: 0d9506e3df294c1ed7da0bf8564ff62b5de96a1f
</commit_message>
<xml_diff>
--- a/src/analysis/tax_transfer_funcs/test_tax_transfers/test_data/test_dfs_alg2.xlsx
+++ b/src/analysis/tax_transfer_funcs/test_tax_transfers/test_data/test_dfs_alg2.xlsx
@@ -91,9 +91,6 @@
     <t>alg2_kdu</t>
   </si>
   <si>
-    <t>divdy</t>
-  </si>
-  <si>
     <t>alg2_ek</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>pid</t>
+  </si>
+  <si>
+    <t>hh_wealth</t>
   </si>
 </sst>
 </file>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI20" sqref="AI20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>12</v>
@@ -573,10 +573,10 @@
         <v>11</v>
       </c>
       <c r="I1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>34</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>35</v>
       </c>
       <c r="K1" s="13" t="s">
         <v>9</v>
@@ -615,22 +615,22 @@
         <v>20</v>
       </c>
       <c r="W1" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X1" s="13" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="Y1" s="13" t="s">
         <v>2</v>
       </c>
       <c r="Z1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="AA1" s="14" t="s">
-        <v>30</v>
-      </c>
       <c r="AB1" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AC1" s="13" t="s">
         <v>22</v>
@@ -645,22 +645,22 @@
         <v>21</v>
       </c>
       <c r="AG1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="AH1" s="13" t="s">
-        <v>27</v>
-      </c>
       <c r="AI1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" s="13" t="s">
-        <v>32</v>
-      </c>
       <c r="AK1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="13" t="s">
         <v>36</v>
-      </c>
-      <c r="AL1" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="AM1" s="13" t="s">
         <v>10</v>
@@ -3018,7 +3018,7 @@
         <v>400</v>
       </c>
       <c r="AF20" s="26">
-        <f>IF(X20/0.025&gt;$AI$20+$AI$21,0,AD20+AE20)</f>
+        <f>IF(X20&gt;$AI$20+$AI$21,0,AD20+AE20)</f>
         <v>1046.2</v>
       </c>
       <c r="AG20">

</xml_diff>